<commit_message>
fix wrong parent for dpv:hasRule properties
- fixes (source, RDF, HTML) dpv:hasRule where child properties instead
  had dpv:Rule as the parent
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/rules.xlsx
+++ b/documentation-generator/vocab_csv/rules.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>Term</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>dpv:Permission</t>
+  </si>
+  <si>
+    <t>dpv:hasRule</t>
   </si>
   <si>
     <t>hasProhibition</t>
@@ -3740,7 +3743,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -3773,22 +3776,22 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -3821,22 +3824,22 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>

</xml_diff>